<commit_message>
Add query.ts to parse query string as conditions
</commit_message>
<xml_diff>
--- a/test_files/us-stock-holiday.xlsx
+++ b/test_files/us-stock-holiday.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuleidong/Me/goodrelay/gr.api.sheet/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F9F3E8EA-60B7-FF49-AB38-69FD9CFBB27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7999955E-3C7E-B344-9740-C7D41BD0C9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="1800" windowWidth="28240" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="us-stock-holiday" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateCount="0" iterateDelta="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
@@ -26,21 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="112" uniqueCount="18">
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>day</t>
-  </si>
-  <si>
-    <t>exchange</t>
-  </si>
-  <si>
-    <t>holiday</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
   <si>
     <t>NYSE</t>
   </si>
@@ -79,6 +64,26 @@
   </si>
   <si>
     <t>Washington’s Birthday</t>
+  </si>
+  <si>
+    <t>ID</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Day</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Exchange</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Holiday</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1061,7 +1066,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1074,19 +1079,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1097,13 +1102,13 @@
         <v>20170102</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1114,10 +1119,10 @@
         <v>20170116</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -1129,10 +1134,10 @@
         <v>20170220</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -1144,10 +1149,10 @@
         <v>20170414</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E5" s="3"/>
     </row>
@@ -1159,10 +1164,10 @@
         <v>20170529</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E6" s="3"/>
     </row>
@@ -1174,10 +1179,10 @@
         <v>20170704</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -1189,10 +1194,10 @@
         <v>20170904</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E8" s="3"/>
     </row>
@@ -1204,10 +1209,10 @@
         <v>20171123</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E9" s="3"/>
     </row>
@@ -1219,10 +1224,10 @@
         <v>20171225</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -1234,10 +1239,10 @@
         <v>20180101</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3"/>
     </row>
@@ -1249,10 +1254,10 @@
         <v>20180115</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -1264,10 +1269,10 @@
         <v>20180219</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -1279,10 +1284,10 @@
         <v>20180330</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3"/>
     </row>
@@ -1294,10 +1299,10 @@
         <v>20180528</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -1309,10 +1314,10 @@
         <v>20180704</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -1324,10 +1329,10 @@
         <v>20180903</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -1339,10 +1344,10 @@
         <v>20181122</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E18" s="3"/>
     </row>
@@ -1354,10 +1359,10 @@
         <v>20181225</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E19" s="3"/>
     </row>
@@ -1369,10 +1374,10 @@
         <v>20190101</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E20" s="3"/>
     </row>
@@ -1384,10 +1389,10 @@
         <v>20190121</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E21" s="3"/>
     </row>
@@ -1399,10 +1404,10 @@
         <v>20190218</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -1414,10 +1419,10 @@
         <v>20190419</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E23" s="3"/>
     </row>
@@ -1429,10 +1434,10 @@
         <v>20190527</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E24" s="3"/>
     </row>
@@ -1444,10 +1449,10 @@
         <v>20190704</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -1459,10 +1464,10 @@
         <v>20190902</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E26" s="3"/>
     </row>
@@ -1474,10 +1479,10 @@
         <v>20191128</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3"/>
     </row>
@@ -1489,10 +1494,10 @@
         <v>20191225</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E28" s="3"/>
     </row>
@@ -1504,10 +1509,10 @@
         <v>20200101</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E29" s="3"/>
     </row>
@@ -1519,10 +1524,10 @@
         <v>20200120</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E30" s="3"/>
     </row>
@@ -1534,10 +1539,10 @@
         <v>20200217</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E31" s="3"/>
     </row>
@@ -1549,10 +1554,10 @@
         <v>20200410</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E32" s="3"/>
     </row>
@@ -1564,10 +1569,10 @@
         <v>20200525</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E33" s="3"/>
     </row>
@@ -1579,10 +1584,10 @@
         <v>20200703</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E34" s="3"/>
     </row>
@@ -1594,10 +1599,10 @@
         <v>20200907</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E35" s="3"/>
     </row>
@@ -1609,10 +1614,10 @@
         <v>20201126</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E36" s="3"/>
     </row>
@@ -1624,10 +1629,10 @@
         <v>20201225</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E37" s="3"/>
     </row>
@@ -1639,10 +1644,10 @@
         <v>20210101</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E38" s="3"/>
     </row>
@@ -1654,10 +1659,10 @@
         <v>20210118</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E39" s="3"/>
     </row>
@@ -1669,10 +1674,10 @@
         <v>20210215</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E40" s="3"/>
     </row>
@@ -1684,10 +1689,10 @@
         <v>20210402</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E41" s="3"/>
     </row>
@@ -1699,10 +1704,10 @@
         <v>20210531</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E42" s="3"/>
     </row>
@@ -1714,10 +1719,10 @@
         <v>20210705</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E43" s="3"/>
     </row>
@@ -1729,10 +1734,10 @@
         <v>20210906</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E44" s="3"/>
     </row>
@@ -1744,10 +1749,10 @@
         <v>20211125</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E45" s="3"/>
     </row>
@@ -1759,10 +1764,10 @@
         <v>20211224</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="E46" s="3"/>
     </row>
@@ -1774,10 +1779,10 @@
         <v>20220117</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E47" s="3"/>
     </row>
@@ -1789,10 +1794,10 @@
         <v>20220221</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E48" s="3"/>
     </row>
@@ -1804,10 +1809,10 @@
         <v>20220415</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E49" s="3"/>
     </row>
@@ -1819,10 +1824,10 @@
         <v>20220530</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="E50" s="3"/>
     </row>
@@ -1834,10 +1839,10 @@
         <v>20220704</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E51" s="3"/>
     </row>
@@ -1849,10 +1854,10 @@
         <v>20220905</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E52" s="3"/>
     </row>
@@ -1864,10 +1869,10 @@
         <v>20221124</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E53" s="3"/>
     </row>
@@ -1879,10 +1884,10 @@
         <v>20221226</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E54" s="3"/>
     </row>

</xml_diff>